<commit_message>
Update diary-junxian-chen.xlsx 0206 (#272)
</commit_message>
<xml_diff>
--- a/diaries/diary-junxian-chen.xlsx
+++ b/diaries/diary-junxian-chen.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joxon\Documents\_Repos\swe265p-reveng\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D3F36F-9A1C-40E7-9A06-4E45CFAD8591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F6D76-E926-427C-BC59-090C00564AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7248" yWindow="744" windowWidth="23040" windowHeight="6900" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="78">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -308,6 +307,50 @@
     <t>A good UML class diagram may help us better understand the project. Here we adopted a top-bottom method to visualize our class diagram which made it easy to read.
 It was interesting to know that someone named their variables with the terms from Lord of Rings
 Also it is necessary to learn how to use Maven or Gradle. Our team should read more official documentations.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>8-9pm</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zihua</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decide features for homework 2.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Because we cannot duplicate the features that we have done in homework 1, it took a long time to decide our goals.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>We decided one feature which is "Adding more query methods".</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not so good</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10am-2pm</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zihua, Wenchia</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decide anther feature and finish writing our report.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>We decided another one feature which is "Adding more encryption methods". The first feature is easy to deal with. But the second one was involved with some C++ native functions which were hard to understand. But we did our best.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Because Wenchia had an important interview this morning so we postponed our group activity. We worked hard together and finished the homework in time.</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -843,9 +886,9 @@
   <dimension ref="A1:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2820" topLeftCell="A16" activePane="bottomLeft"/>
+      <pane ySplit="2820" topLeftCell="A19" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="A1:XFD9"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1196,23 +1239,51 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="2"/>
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>20200204</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="4" customFormat="1" ht="93.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20200206</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>

</xml_diff>

<commit_message>
Update diary-junxian-chen.xlsx 20200219 (#335)
</commit_message>
<xml_diff>
--- a/diaries/diary-junxian-chen.xlsx
+++ b/diaries/diary-junxian-chen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joxon\Documents\_Repos\swe265p-reveng\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD847BA-BB36-4681-A386-B3384135841C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3798F24B-B826-454A-9761-E52524C7DBA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="744" windowWidth="23040" windowHeight="6900" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -373,6 +373,59 @@
   </si>
   <si>
     <t xml:space="preserve">The midterm seems hard so I better get prepared. </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Midterm;
+2. Learn more KEPs;
+3. Learn about Stakeholders.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 KEPs learned:
+1. Prioritize Stakeholders;
+2. Move along levels of abstraction;
+3. Do something else.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>The exam has a theoretical part and a pratical part. I think the theoretical part was not difficult if you have gone through all the slides and memorized some key concepts. However, the practical part of analyzing the pacman code seemed tricky because the question might have different interpretations. In the first question we were asked to use SimpleUML to draw a diagram of classes DIRECTLY related to the Game class and the SinglePlayerGame class without writing fields and constructors (what about methods?). Here the word DIRECTLY did not have a clear definition. In the next question we had to purpose some beacons, which also varied from person to person. So I was confused if I really understood what the questions wanted.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3:00-3:20pm</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kaj, Wenchia</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>To discuss what we can do to improve our report for homework 2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:00-11:00am</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>We learned that the features picked by us in the report were not essential in the project. And we were asked to what was inside the realm-java and figure out was it really just a wrapper or something more.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>To report our discovery to Kaj and see what we can do</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>It was very frustrating to know why our homework got such a low score. We even thought about switching to different projects but knew that was not likely to happen. So instead we had to dig into realm-core written in C++, making the whole process more challenging. We might not be on the right track of searching essential features because they are not even implemented in realm-java.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">We still cannot confirm whether realm-java is only a wrapper or something more. But we received suggestions from Kaj that we should investigate what realm-java provides differently from the other databases like SQLite. </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>We thought we should know how to use realm-java in real projects first, then try to understand what makes realm-java stands out among all these database libraries. If it is just nothing new, then we will have to research essential features like querying in realm-core.</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -907,10 +960,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2820" topLeftCell="A20" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2820" topLeftCell="A24" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="A1:XFD9"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1330,32 +1383,74 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="2"/>
+    <row r="23" spans="1:7" s="4" customFormat="1" ht="399.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>20200213</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="232.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>20200218</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="4" customFormat="1" ht="154.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>20200219</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>

</xml_diff>